<commit_message>
Updated image_explorer_rules.csv to correct file
</commit_message>
<xml_diff>
--- a/code/validator/www/microplastic_images/image_explorer_rules.xlsx
+++ b/code/validator/www/microplastic_images/image_explorer_rules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahsherrod/Documents/MooreResearchRepository/Microplastic_Data_Portal/code/validator/www/microplastic_images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FE07950-9E42-4A44-9665-6923C6A0A121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FC4E34E-90C6-8D4A-916F-451867C5124E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -591,7 +591,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>